<commit_message>
Added model stats for water model with data from prior stream study
The 16S rRNA water ASVs UOG dataset was used with data from Deaven et al. 2021 (https://pubmed.ncbi.nlm.nih.gov/33397693/, BioProject PRJNA707295) to generated an additional random forest model based on the shared ASVs between the two datasets.
</commit_message>
<xml_diff>
--- a/S.Table8.xlsx
+++ b/S.Table8.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pacea\OneDrive\Documents\GitHub\MultiomicsFrackingSupplemental\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\Jeremy\Documents\RW\May.2022\fracking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE23EA86-B7DA-412D-B073-7E6E87AE4D60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAF4D39E-E7BE-4957-A213-C7A01F3BDE32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3135" yWindow="1905" windowWidth="21600" windowHeight="11385" xr2:uid="{02E1F8EF-2486-4C34-BF46-B0E30763AA5A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{02E1F8EF-2486-4C34-BF46-B0E30763AA5A}"/>
   </bookViews>
   <sheets>
     <sheet name="S.Table8" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="44">
   <si>
     <t>Model input</t>
   </si>
@@ -163,6 +163,9 @@
   </si>
   <si>
     <t>Supplemental Table 8: Random forest models accuracy and area under the curve (AUC)</t>
+  </si>
+  <si>
+    <t>16S rRNA water ASVs, UOG with data from Deaven et al. 2021 (https://pubmed.ncbi.nlm.nih.gov/33397693/, BioProject PRJNA707295)</t>
   </si>
 </sst>
 </file>
@@ -210,11 +213,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -532,9 +536,11 @@
   <sheetPr codeName="Sheet77">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H36"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -916,7 +922,7 @@
         <v>0.64080000000000004</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>22</v>
       </c>
@@ -942,7 +948,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>23</v>
       </c>
@@ -968,471 +974,498 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" s="4">
+        <v>0.33377449682691201</v>
+      </c>
+      <c r="C19" s="4">
+        <v>0.27558238890000702</v>
+      </c>
+      <c r="D19" s="4">
+        <v>0.34333333333333299</v>
+      </c>
+      <c r="E19" s="4">
+        <v>0.99016171307957501</v>
+      </c>
+      <c r="F19" s="4">
+        <v>0.94022968848970401</v>
+      </c>
+      <c r="G19" s="4">
+        <v>0.87754545454545496</v>
+      </c>
+      <c r="H19" s="4">
+        <v>0.76307142857142896</v>
+      </c>
+      <c r="I19" s="4"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>24</v>
       </c>
-      <c r="B19">
+      <c r="B20">
         <v>0.99988585287241505</v>
       </c>
-      <c r="C19">
+      <c r="C20">
         <v>0.99960842064307798</v>
       </c>
-      <c r="D19">
+      <c r="D20">
         <v>0.99262499999999998</v>
       </c>
-      <c r="E19">
+      <c r="E20">
         <v>0.54206793611779402</v>
       </c>
-      <c r="F19">
+      <c r="F20">
         <v>0.59154943773953395</v>
       </c>
-      <c r="G19">
+      <c r="G20">
         <v>0.60199999999999998</v>
       </c>
-      <c r="H19">
+      <c r="H20">
         <v>0.91449999999999998</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>25</v>
       </c>
-      <c r="B20">
+      <c r="B21">
         <v>0.99736880811642803</v>
       </c>
-      <c r="C20">
+      <c r="C21">
         <v>0.99391433468986301</v>
       </c>
-      <c r="D20">
+      <c r="D21">
         <v>0.96220000000000006</v>
       </c>
-      <c r="E20">
+      <c r="E21">
         <v>0.87914215345327795</v>
       </c>
-      <c r="F20">
+      <c r="F21">
         <v>0.85235041142802204</v>
       </c>
-      <c r="G20">
+      <c r="G21">
         <v>0.78200000000000003</v>
       </c>
-      <c r="H20">
+      <c r="H21">
         <v>0.91071428571428603</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>26</v>
       </c>
-      <c r="B21">
+      <c r="B22">
         <v>0.97076854911681898</v>
       </c>
-      <c r="C21">
+      <c r="C22">
         <v>0.95399362744453597</v>
       </c>
-      <c r="D21">
+      <c r="D22">
         <v>0.88800000000000001</v>
       </c>
-      <c r="E21">
+      <c r="E22">
         <v>0.99943839478293195</v>
       </c>
-      <c r="F21">
+      <c r="F22">
         <v>0.99884473044685496</v>
       </c>
-      <c r="G21">
+      <c r="G22">
         <v>0.98099999999999998</v>
       </c>
-      <c r="H21">
+      <c r="H22">
         <v>0.9345</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>27</v>
       </c>
-      <c r="B22">
+      <c r="B23">
         <v>0.99892352046431099</v>
       </c>
-      <c r="C22">
+      <c r="C23">
         <v>0.99693954204414303</v>
       </c>
-      <c r="D22">
+      <c r="D23">
         <v>0.974833333333333</v>
       </c>
-      <c r="E22">
+      <c r="E23">
         <v>0.80029961995913301</v>
       </c>
-      <c r="F22">
+      <c r="F23">
         <v>0.81629712781363695</v>
       </c>
-      <c r="G22">
+      <c r="G23">
         <v>0.76200000000000001</v>
       </c>
-      <c r="H22">
+      <c r="H23">
         <v>0.92162500000000003</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>28</v>
       </c>
-      <c r="B23">
+      <c r="B24">
         <v>0.95919234602928405</v>
       </c>
-      <c r="C23">
+      <c r="C24">
         <v>0.92997231297468896</v>
       </c>
-      <c r="D23">
+      <c r="D24">
         <v>0.86475000000000002</v>
       </c>
-      <c r="E23">
+      <c r="E24">
         <v>0.99321805493956095</v>
       </c>
-      <c r="F23">
+      <c r="F24">
         <v>0.98821412620608495</v>
       </c>
-      <c r="G23">
+      <c r="G24">
         <v>0.94750000000000001</v>
       </c>
-      <c r="H23">
+      <c r="H24">
         <v>0.89233333333333298</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>29</v>
       </c>
-      <c r="B24">
+      <c r="B25">
         <v>0.64904829425934896</v>
       </c>
-      <c r="C24">
+      <c r="C25">
         <v>0.66405825985450795</v>
       </c>
-      <c r="D24">
+      <c r="D25">
         <v>0.59250000000000003</v>
       </c>
-      <c r="E24">
+      <c r="E25">
         <v>0.99999988210756297</v>
       </c>
-      <c r="F24">
+      <c r="F25">
         <v>0.99999968434418396</v>
       </c>
-      <c r="G24">
+      <c r="G25">
         <v>0.99950000000000006</v>
       </c>
-      <c r="H24">
+      <c r="H25">
         <v>0.79600000000000004</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>30</v>
       </c>
-      <c r="B25">
+      <c r="B26">
         <v>0.99997489858553601</v>
       </c>
-      <c r="C25">
+      <c r="C26">
         <v>0.99993962418234505</v>
       </c>
-      <c r="D25">
+      <c r="D26">
         <v>0.997</v>
       </c>
-      <c r="E25">
+      <c r="E26">
         <v>0.17945288880674601</v>
       </c>
-      <c r="F25" s="2">
+      <c r="F26" s="2">
         <v>2.8786659364027398E-7</v>
       </c>
-      <c r="G25" s="3">
+      <c r="G26" s="3">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="H25">
+      <c r="H26">
         <v>0.79769999999999996</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>31</v>
       </c>
-      <c r="B26">
+      <c r="B27">
         <v>0.98138031413040805</v>
       </c>
-      <c r="C26">
+      <c r="C27">
         <v>0.97322787364539498</v>
       </c>
-      <c r="D26">
+      <c r="D27">
         <v>0.9234</v>
       </c>
-      <c r="E26">
+      <c r="E27">
         <v>0.25271992997109999</v>
       </c>
-      <c r="F26">
+      <c r="F27">
         <v>4.0590211215430903E-2</v>
       </c>
-      <c r="G26">
+      <c r="G27">
         <v>0.11799999999999999</v>
       </c>
-      <c r="H26">
+      <c r="H27">
         <v>0.69328571428571395</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>32</v>
       </c>
-      <c r="B27">
+      <c r="B28">
         <v>0.39534565525096099</v>
       </c>
-      <c r="C27">
+      <c r="C28">
         <v>0.37227236428965199</v>
       </c>
-      <c r="D27">
+      <c r="D28">
         <v>0.39950000000000002</v>
       </c>
-      <c r="E27">
+      <c r="E28">
         <v>0.92394500146078495</v>
       </c>
-      <c r="F27">
+      <c r="F28">
         <v>0.91302815295478701</v>
       </c>
-      <c r="G27">
+      <c r="G28">
         <v>0.83299999999999996</v>
       </c>
-      <c r="H27">
+      <c r="H28">
         <v>0.61624999999999996</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>33</v>
       </c>
-      <c r="B28">
+      <c r="B29">
         <v>0.99986508301076704</v>
       </c>
-      <c r="C28">
+      <c r="C29">
         <v>0.99972790968190095</v>
       </c>
-      <c r="D28">
+      <c r="D29">
         <v>0.99316666666666698</v>
       </c>
-      <c r="E28">
+      <c r="E29">
         <v>0.219007110831098</v>
       </c>
-      <c r="F28">
+      <c r="F29">
         <v>6.0863911891125303E-4</v>
       </c>
-      <c r="G28">
+      <c r="G29">
         <v>1.35E-2</v>
       </c>
-      <c r="H28">
+      <c r="H29">
         <v>0.74824999999999997</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>34</v>
       </c>
-      <c r="B29">
+      <c r="B30">
         <v>0.78314577378419703</v>
       </c>
-      <c r="C29">
+      <c r="C30">
         <v>0.81093656232692901</v>
       </c>
-      <c r="D29">
+      <c r="D30">
         <v>0.75424999999999998</v>
       </c>
-      <c r="E29">
+      <c r="E30">
         <v>0.57763491060925198</v>
       </c>
-      <c r="F29">
+      <c r="F30">
         <v>0.60616451396737803</v>
       </c>
-      <c r="G29">
+      <c r="G30">
         <v>0.59250000000000003</v>
       </c>
-      <c r="H29">
+      <c r="H30">
         <v>0.70033333333333303</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>35</v>
       </c>
-      <c r="B30">
+      <c r="B31">
         <v>0.28866272690490002</v>
       </c>
-      <c r="C30">
+      <c r="C31">
         <v>0.19709009767022601</v>
       </c>
-      <c r="D30">
+      <c r="D31">
         <v>0.28050000000000003</v>
       </c>
-      <c r="E30">
+      <c r="E31">
         <v>1</v>
       </c>
-      <c r="F30">
+      <c r="F31">
         <v>1</v>
       </c>
-      <c r="G30">
+      <c r="G31">
         <v>1</v>
       </c>
-      <c r="H30">
+      <c r="H31">
         <v>0.64024999999999999</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>36</v>
       </c>
-      <c r="B31">
+      <c r="B32">
         <v>0.98739052820643303</v>
       </c>
-      <c r="C31">
+      <c r="C32">
         <v>0.97419418193114204</v>
       </c>
-      <c r="D31">
+      <c r="D32">
         <v>0.94587500000000002</v>
       </c>
-      <c r="E31">
+      <c r="E32">
         <v>0.24086787751312599</v>
       </c>
-      <c r="F31">
+      <c r="F32">
         <v>0.10330359168936</v>
       </c>
-      <c r="G31">
+      <c r="G32">
         <v>0.1835</v>
       </c>
-      <c r="H31">
+      <c r="H32">
         <v>0.79339999999999999</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>37</v>
-      </c>
-      <c r="B32">
-        <v>0.96136587482897495</v>
-      </c>
-      <c r="C32">
-        <v>0.94396852270245102</v>
-      </c>
-      <c r="D32">
-        <v>0.88</v>
-      </c>
-      <c r="E32">
-        <v>0.403586228883757</v>
-      </c>
-      <c r="F32">
-        <v>0.39243571373859798</v>
-      </c>
-      <c r="G32">
-        <v>0.4365</v>
-      </c>
-      <c r="H32">
-        <v>0.753285714285714</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B33">
-        <v>0.70434986780244002</v>
+        <v>0.96136587482897495</v>
       </c>
       <c r="C33">
-        <v>0.72962933699079002</v>
+        <v>0.94396852270245102</v>
       </c>
       <c r="D33">
-        <v>0.70599999999999996</v>
+        <v>0.88</v>
       </c>
       <c r="E33">
-        <v>0.98938436011613995</v>
+        <v>0.403586228883757</v>
       </c>
       <c r="F33">
-        <v>0.98224599190974804</v>
+        <v>0.39243571373859798</v>
       </c>
       <c r="G33">
-        <v>0.92649999999999999</v>
+        <v>0.4365</v>
       </c>
       <c r="H33">
-        <v>0.81625000000000003</v>
+        <v>0.753285714285714</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B34">
-        <v>0.99940272524667295</v>
+        <v>0.70434986780244002</v>
       </c>
       <c r="C34">
-        <v>0.99811561411896499</v>
+        <v>0.72962933699079002</v>
       </c>
       <c r="D34">
-        <v>0.97550000000000003</v>
+        <v>0.70599999999999996</v>
       </c>
       <c r="E34">
-        <v>0.983549926321304</v>
+        <v>0.98938436011613995</v>
       </c>
       <c r="F34">
-        <v>0.97278056878341601</v>
+        <v>0.98224599190974804</v>
       </c>
       <c r="G34">
-        <v>0.91</v>
+        <v>0.92649999999999999</v>
       </c>
       <c r="H34">
-        <v>0.95912500000000001</v>
+        <v>0.81625000000000003</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B35">
-        <v>0.99515160644496903</v>
+        <v>0.99940272524667295</v>
       </c>
       <c r="C35">
-        <v>0.99011430064053896</v>
+        <v>0.99811561411896499</v>
       </c>
       <c r="D35">
-        <v>0.95</v>
+        <v>0.97550000000000003</v>
       </c>
       <c r="E35">
-        <v>0.99977501239409095</v>
+        <v>0.983549926321304</v>
       </c>
       <c r="F35">
-        <v>0.99950799057434003</v>
+        <v>0.97278056878341601</v>
       </c>
       <c r="G35">
-        <v>0.98799999999999999</v>
+        <v>0.91</v>
       </c>
       <c r="H35">
-        <v>0.962666666666667</v>
+        <v>0.95912500000000001</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>40</v>
+      </c>
+      <c r="B36">
+        <v>0.99515160644496903</v>
+      </c>
+      <c r="C36">
+        <v>0.99011430064053896</v>
+      </c>
+      <c r="D36">
+        <v>0.95</v>
+      </c>
+      <c r="E36">
+        <v>0.99977501239409095</v>
+      </c>
+      <c r="F36">
+        <v>0.99950799057434003</v>
+      </c>
+      <c r="G36">
+        <v>0.98799999999999999</v>
+      </c>
+      <c r="H36">
+        <v>0.962666666666667</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>41</v>
       </c>
-      <c r="B36">
+      <c r="B37">
         <v>0.99148026012351897</v>
       </c>
-      <c r="C36">
+      <c r="C37">
         <v>0.98219474725413203</v>
       </c>
-      <c r="D36">
+      <c r="D37">
         <v>0.93300000000000005</v>
       </c>
-      <c r="E36">
+      <c r="E37">
         <v>0.99990433264448297</v>
       </c>
-      <c r="F36">
+      <c r="F37">
         <v>0.99963668173187703</v>
       </c>
-      <c r="G36">
+      <c r="G37">
         <v>0.98950000000000005</v>
       </c>
-      <c r="H36">
+      <c r="H37">
         <v>0.96125000000000005</v>
       </c>
     </row>

</xml_diff>